<commit_message>
Further work on betting odds strategy
</commit_message>
<xml_diff>
--- a/data/f1_betting_odds.xlsx
+++ b/data/f1_betting_odds.xlsx
@@ -1,6 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
@@ -129,12 +132,33 @@
   <si>
     <t>Odds_Quali</t>
   </si>
+  <si>
+    <t>66/1</t>
+  </si>
+  <si>
+    <t>40/1</t>
+  </si>
+  <si>
+    <t>80/1</t>
+  </si>
+  <si>
+    <t>150/1</t>
+  </si>
+  <si>
+    <t>400/1</t>
+  </si>
+  <si>
+    <t>200/1</t>
+  </si>
+  <si>
+    <t>500/1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <numFmts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" mc:Ignorable="x14ac">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
@@ -143,6 +167,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -184,9 +209,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -515,10 +553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="topLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <cols>
+    <col min="5" max="5" style="5"/>
     <col min="6" max="6" width="15.74" customWidth="1"/>
     <col min="7" max="7" width="14.12" customWidth="1"/>
   </cols>
@@ -536,7 +575,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -559,6 +598,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" s="4">
+        <v>46027</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -573,6 +615,9 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3" s="4">
+        <v>46030</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -587,6 +632,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" s="4">
+        <v>46025</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -601,6 +649,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5" s="4">
+        <v>46033</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -615,6 +666,9 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" s="4">
+        <v>46125</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -629,6 +683,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -643,6 +700,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -657,6 +717,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9" s="4">
+        <v>46044</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -671,6 +734,9 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -685,6 +751,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -699,6 +768,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -713,6 +785,9 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -727,6 +802,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14" s="4">
+        <v>46036</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -741,6 +819,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -755,6 +836,9 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -769,6 +853,9 @@
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -783,6 +870,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -797,6 +887,9 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -811,6 +904,9 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -825,6 +921,9 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -839,6 +938,9 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -853,126 +955,8 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24">
-        <v>2026</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25">
-        <v>2026</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26">
-        <v>2026</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27">
-        <v>2026</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28">
-        <v>2026</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29">
-        <v>2026</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30">
-        <v>2026</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31">
-        <v>2026</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32">
-        <v>2026</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33">
-        <v>2026</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>2026</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
+      <c r="E23" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script to select team based on betting odds
</commit_message>
<xml_diff>
--- a/data/f1_betting_odds.xlsx
+++ b/data/f1_betting_odds.xlsx
@@ -152,6 +152,36 @@
   </si>
   <si>
     <t>500/1</t>
+  </si>
+  <si>
+    <t>'5/1</t>
+  </si>
+  <si>
+    <t>"5/1"</t>
+  </si>
+  <si>
+    <t>5/1</t>
+  </si>
+  <si>
+    <t>8/1</t>
+  </si>
+  <si>
+    <t>3/1</t>
+  </si>
+  <si>
+    <t>11/1</t>
+  </si>
+  <si>
+    <t>13/4</t>
+  </si>
+  <si>
+    <t>22/1</t>
+  </si>
+  <si>
+    <t>14/1</t>
+  </si>
+  <si>
+    <t>200/2</t>
   </si>
 </sst>
 </file>
@@ -209,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -225,6 +255,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -553,13 +591,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" sqref="J31"/>
+      <selection pane="topLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col min="5" max="5" style="5"/>
-    <col min="6" max="6" width="15.74" customWidth="1"/>
-    <col min="7" max="7" width="14.12" customWidth="1"/>
+    <col min="6" max="6" width="15.74" style="10" customWidth="1"/>
+    <col min="7" max="7" width="14.12" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -578,10 +616,10 @@
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -598,9 +636,10 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
-        <v>46027</v>
-      </c>
+      <c r="E2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -615,9 +654,10 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
-        <v>46030</v>
-      </c>
+      <c r="E3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -632,9 +672,10 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
-        <v>46025</v>
-      </c>
+      <c r="E4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -649,9 +690,10 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
-        <v>46033</v>
-      </c>
+      <c r="E5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -666,9 +708,10 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
-        <v>46125</v>
-      </c>
+      <c r="E6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -683,9 +726,10 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="G7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -700,9 +744,10 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="10" t="s">
         <v>41</v>
       </c>
+      <c r="G8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -717,9 +762,10 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="4">
-        <v>46044</v>
-      </c>
+      <c r="E9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -734,9 +780,10 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="G10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -751,9 +798,10 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="G11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -768,9 +816,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="G12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -785,9 +834,10 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
+      <c r="G13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -802,9 +852,10 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
-        <v>46036</v>
-      </c>
+      <c r="E14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -819,9 +870,10 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="G15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -836,9 +888,10 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="G16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -853,9 +906,10 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="G17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -870,9 +924,10 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="G18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -887,9 +942,10 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="G19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -904,9 +960,10 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="G20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -921,9 +978,10 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="10" t="s">
         <v>44</v>
       </c>
+      <c r="G21" s="10"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -938,9 +996,10 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="10" t="s">
         <v>46</v>
       </c>
+      <c r="G22" s="10"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -955,9 +1014,10 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="10" t="s">
         <v>46</v>
       </c>
+      <c r="G23" s="10"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
Tweaks to betting odds starting selection
</commit_message>
<xml_diff>
--- a/data/f1_betting_odds.xlsx
+++ b/data/f1_betting_odds.xlsx
@@ -182,6 +182,48 @@
   </si>
   <si>
     <t>200/2</t>
+  </si>
+  <si>
+    <t>11:4</t>
+  </si>
+  <si>
+    <t>7:2</t>
+  </si>
+  <si>
+    <t>8:1</t>
+  </si>
+  <si>
+    <t>11:1</t>
+  </si>
+  <si>
+    <t>12:1</t>
+  </si>
+  <si>
+    <t>20:1</t>
+  </si>
+  <si>
+    <t>33:1</t>
+  </si>
+  <si>
+    <t>75:1</t>
+  </si>
+  <si>
+    <t>80:1</t>
+  </si>
+  <si>
+    <t>100:1</t>
+  </si>
+  <si>
+    <t>200:1</t>
+  </si>
+  <si>
+    <t>250:1</t>
+  </si>
+  <si>
+    <t>400:1</t>
+  </si>
+  <si>
+    <t>500:1</t>
   </si>
 </sst>
 </file>
@@ -591,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -637,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -655,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -673,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -691,7 +733,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -709,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -727,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G7" s="10"/>
     </row>
@@ -745,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="G8" s="10"/>
     </row>
@@ -763,7 +805,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G9" s="10"/>
     </row>
@@ -781,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -799,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="G11" s="10"/>
     </row>
@@ -817,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G12" s="10"/>
     </row>
@@ -835,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="G13" s="10"/>
     </row>
@@ -853,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G14" s="10"/>
     </row>
@@ -871,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -889,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -907,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -925,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -943,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -961,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -979,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -997,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -1015,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="G23" s="10"/>
     </row>

</xml_diff>